<commit_message>
analysis with adapated non-food basics, removal of alcoholic drinks, perfected original do files and works on UNHS-2005
</commit_message>
<xml_diff>
--- a/ww-ug/GAPP_RESULTS_WRITE_UP/GAPP-CALCULATIONS.xlsx
+++ b/ww-ug/GAPP_RESULTS_WRITE_UP/GAPP-CALCULATIONS.xlsx
@@ -15,9 +15,128 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>ent</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>difference</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>Urban</t>
+  </si>
+  <si>
+    <t>Central Rural</t>
+  </si>
+  <si>
+    <t>Central Urban</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>Eastern</t>
+  </si>
+  <si>
+    <t>Northern</t>
+  </si>
+  <si>
+    <t>Western</t>
+  </si>
+  <si>
+    <t>Kampala</t>
+  </si>
+  <si>
+    <t>Central 1</t>
+  </si>
+  <si>
+    <t>Central 2</t>
+  </si>
+  <si>
+    <t>East central</t>
+  </si>
+  <si>
+    <t>Mid-Northern</t>
+  </si>
+  <si>
+    <t>North-east</t>
+  </si>
+  <si>
+    <t>West-Nile</t>
+  </si>
+  <si>
+    <t>Mid-Western</t>
+  </si>
+  <si>
+    <t>South-Western</t>
+  </si>
+  <si>
+    <t>ubos</t>
+  </si>
+  <si>
+    <t>ubos-diffs</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>west and central rural</t>
+  </si>
+  <si>
+    <t>east north and central urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rural </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urban </t>
+  </si>
+  <si>
+    <t>central</t>
+  </si>
+  <si>
+    <t>eastern</t>
+  </si>
+  <si>
+    <t>northern</t>
+  </si>
+  <si>
+    <t>western</t>
+  </si>
+  <si>
+    <t>total freq</t>
+  </si>
+  <si>
+    <t>% pov diffs totals</t>
+  </si>
+  <si>
+    <t>contributors</t>
+  </si>
+  <si>
+    <t>total rural</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,13 +144,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6A6A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -98,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -115,6 +265,15 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,102 +586,691 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="8"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>21258</v>
       </c>
-      <c r="B1" s="2">
-        <f>C1-A1</f>
+      <c r="B2" s="2">
+        <f>C2-A2</f>
         <v>10848</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C2" s="2">
         <v>32106</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>21258</v>
-      </c>
-      <c r="B2" s="4">
-        <f t="shared" ref="B2:B8" si="0">C2-A2</f>
-        <v>8314</v>
-      </c>
-      <c r="C2" s="5">
-        <v>29572</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>21258</v>
       </c>
       <c r="B3" s="4">
+        <f t="shared" ref="B3:B9" si="0">C3-A3</f>
+        <v>8314</v>
+      </c>
+      <c r="C3" s="5">
+        <v>29572</v>
+      </c>
+      <c r="E3" s="7">
+        <v>23.3</v>
+      </c>
+      <c r="F3" s="7">
+        <v>23.5</v>
+      </c>
+      <c r="G3">
+        <v>24.5</v>
+      </c>
+      <c r="H3" s="8">
+        <f>F3-E3</f>
+        <v>0.19999999999999929</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="9">
+        <f>F3-G3</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>21258</v>
+      </c>
+      <c r="B4" s="4">
         <f t="shared" si="0"/>
         <v>9427</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C4" s="5">
         <v>30685</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="E4" s="7">
+        <v>26.2</v>
+      </c>
+      <c r="F4" s="7">
+        <v>26.3</v>
+      </c>
+      <c r="G4">
+        <v>27.2</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" ref="H4:H22" si="1">F4-E4</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" ref="J4:J22" si="2">F4-G4</f>
+        <v>-0.89999999999999858</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>21258</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B5" s="4">
         <f t="shared" si="0"/>
         <v>7384</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C5" s="5">
         <v>28642</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="E5" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="F5" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="G5">
+        <v>9.1</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" si="1"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="2"/>
+        <v>-3.8999999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>21258</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="4">
         <f t="shared" si="0"/>
         <v>8976</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C6" s="5">
         <v>30234</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="E6" s="7">
+        <v>20.6</v>
+      </c>
+      <c r="F6" s="7">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <v>13.5</v>
+      </c>
+      <c r="H6" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.6000000000000014</v>
+      </c>
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="2"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>21258</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B7" s="4">
         <f t="shared" si="0"/>
         <v>7689</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C7" s="5">
         <v>28947</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="E7" s="7">
+        <v>2.9</v>
+      </c>
+      <c r="F7" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G7">
+        <v>5.4</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="1"/>
+        <v>1.1999999999999997</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" si="2"/>
+        <v>-1.3000000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>21258</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B8" s="4">
         <f t="shared" si="0"/>
         <v>8735</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C8" s="5">
         <v>29993</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="E8" s="7">
+        <v>14.8</v>
+      </c>
+      <c r="F8" s="7">
+        <v>14.2</v>
+      </c>
+      <c r="G8">
+        <v>10.7</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="1"/>
+        <v>-0.60000000000000142</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="2"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>21258</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B9" s="4">
         <f t="shared" si="0"/>
         <v>6907</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C9" s="5">
         <v>28165</v>
+      </c>
+      <c r="E9" s="7">
+        <v>17.8</v>
+      </c>
+      <c r="F9" s="7">
+        <v>30.3</v>
+      </c>
+      <c r="G9">
+        <v>24.3</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="7">
+        <v>17</v>
+      </c>
+      <c r="F10" s="7">
+        <v>21.6</v>
+      </c>
+      <c r="G10">
+        <v>46.2</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" si="1"/>
+        <v>4.6000000000000014</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="9">
+        <f t="shared" si="2"/>
+        <v>-24.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="7">
+        <v>45.2</v>
+      </c>
+      <c r="F11" s="7">
+        <v>25.4</v>
+      </c>
+      <c r="G11">
+        <v>21.8</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="1"/>
+        <v>-19.800000000000004</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" si="2"/>
+        <v>3.5999999999999979</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="K12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="9">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="K13" s="10">
+        <f>Q15+Q16+Q17+Q18+Q13</f>
+        <v>4171</v>
+      </c>
+      <c r="L13">
+        <f>H13+H16+H17+H18+H19+H20</f>
+        <v>39.799999999999997</v>
+      </c>
+      <c r="M13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q13">
+        <v>809</v>
+      </c>
+      <c r="R13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="7">
+        <v>13.2</v>
+      </c>
+      <c r="F14" s="7">
+        <v>12.9</v>
+      </c>
+      <c r="G14">
+        <v>11.2</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="1"/>
+        <v>-0.29999999999999893</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="9">
+        <f t="shared" si="2"/>
+        <v>1.7000000000000011</v>
+      </c>
+      <c r="K14">
+        <f>((K13/Q21)*100)</f>
+        <v>61.564575645756456</v>
+      </c>
+      <c r="P14" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>1177</v>
+      </c>
+      <c r="T14" s="10">
+        <f>Q18+Q16</f>
+        <v>3058</v>
+      </c>
+      <c r="U14">
+        <f>T14/T23</f>
+        <v>0.55049504950495054</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="7">
+        <v>22.3</v>
+      </c>
+      <c r="F15" s="7">
+        <v>20.5</v>
+      </c>
+      <c r="G15">
+        <v>13.6</v>
+      </c>
+      <c r="H15" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.8000000000000007</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="9">
+        <f t="shared" si="2"/>
+        <v>6.9</v>
+      </c>
+      <c r="P15" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q15">
+        <v>132</v>
+      </c>
+      <c r="R15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="7">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="F16" s="7">
+        <v>27.4</v>
+      </c>
+      <c r="G16">
+        <v>21.4</v>
+      </c>
+      <c r="H16" s="8">
+        <f t="shared" si="1"/>
+        <v>10.799999999999997</v>
+      </c>
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="9">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="P16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="17" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="7">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="F17" s="7">
+        <v>32.6</v>
+      </c>
+      <c r="G17">
+        <v>26.5</v>
+      </c>
+      <c r="H17" s="8">
+        <f t="shared" si="1"/>
+        <v>13.700000000000003</v>
+      </c>
+      <c r="I17" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="9">
+        <f t="shared" si="2"/>
+        <v>6.1000000000000014</v>
+      </c>
+      <c r="P17" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q17">
+        <v>172</v>
+      </c>
+      <c r="R17" t="s">
+        <v>32</v>
+      </c>
+      <c r="T17" s="10">
+        <f>Q17+Q18</f>
+        <v>1956</v>
+      </c>
+      <c r="V17">
+        <f>T17/Q21</f>
+        <v>0.28870848708487085</v>
+      </c>
+    </row>
+    <row r="18" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="7">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F18" s="7">
+        <v>13.9</v>
+      </c>
+      <c r="G18">
+        <v>40.4</v>
+      </c>
+      <c r="H18" s="8">
+        <f t="shared" si="1"/>
+        <v>3.7000000000000011</v>
+      </c>
+      <c r="I18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="9">
+        <f t="shared" si="2"/>
+        <v>-26.5</v>
+      </c>
+      <c r="P18" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="19" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="7">
+        <v>54.8</v>
+      </c>
+      <c r="F19" s="7">
+        <v>60.4</v>
+      </c>
+      <c r="G19">
+        <v>75.8</v>
+      </c>
+      <c r="H19" s="8">
+        <f t="shared" si="1"/>
+        <v>5.6000000000000014</v>
+      </c>
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="9">
+        <f t="shared" si="2"/>
+        <v>-15.399999999999999</v>
+      </c>
+      <c r="P19" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q19">
+        <v>107</v>
+      </c>
+      <c r="R19" t="s">
+        <v>33</v>
+      </c>
+      <c r="T19" s="10">
+        <f>Q19+Q20</f>
+        <v>1427</v>
+      </c>
+      <c r="V19">
+        <f>T19/Q21</f>
+        <v>0.21062730627306273</v>
+      </c>
+    </row>
+    <row r="20" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="7">
+        <v>9</v>
+      </c>
+      <c r="F20" s="7">
+        <v>14.2</v>
+      </c>
+      <c r="G20">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="H20" s="8">
+        <f t="shared" si="1"/>
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="9">
+        <f t="shared" si="2"/>
+        <v>-25.500000000000004</v>
+      </c>
+      <c r="P20" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q20" s="10">
+        <v>1320</v>
+      </c>
+      <c r="T20" s="10">
+        <f>Q20+Q14</f>
+        <v>2497</v>
+      </c>
+      <c r="U20">
+        <f>T20/T23</f>
+        <v>0.44950495049504952</v>
+      </c>
+    </row>
+    <row r="21" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="7">
+        <v>47.8</v>
+      </c>
+      <c r="F21" s="7">
+        <v>29.5</v>
+      </c>
+      <c r="G21">
+        <v>25.3</v>
+      </c>
+      <c r="H21" s="8">
+        <f t="shared" si="1"/>
+        <v>-18.299999999999997</v>
+      </c>
+      <c r="I21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="9">
+        <f t="shared" si="2"/>
+        <v>4.1999999999999993</v>
+      </c>
+      <c r="K21" s="10">
+        <f>Q19+Q20+Q14</f>
+        <v>2604</v>
+      </c>
+      <c r="L21">
+        <f>H14+H15+H21+H22</f>
+        <v>-41.599999999999994</v>
+      </c>
+      <c r="M21" t="s">
+        <v>26</v>
+      </c>
+      <c r="P21" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q21" s="10">
+        <v>6775</v>
+      </c>
+    </row>
+    <row r="22" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="7">
+        <v>42.4</v>
+      </c>
+      <c r="F22" s="7">
+        <v>21.2</v>
+      </c>
+      <c r="G22">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="H22" s="8">
+        <f t="shared" si="1"/>
+        <v>-21.2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="9">
+        <f t="shared" si="2"/>
+        <v>2.8000000000000007</v>
+      </c>
+      <c r="K22">
+        <f>((K21/Q21)*100)</f>
+        <v>38.435424354243544</v>
+      </c>
+    </row>
+    <row r="23" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="T23" s="10">
+        <f>Q14+Q16+Q18+Q20</f>
+        <v>5555</v>
+      </c>
+    </row>
+    <row r="24" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="T24" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>